<commit_message>
New manufacturing files after emc  modifications
</commit_message>
<xml_diff>
--- a/AnthC-M1R1/BOM esp32 Core  V-0.1.xlsx
+++ b/AnthC-M1R1/BOM esp32 Core  V-0.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\KiCad\Anthilla\esp32 Core  V-0.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doen_\Documents\Working\Anthilla\esp32 Core  V-0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77B4620-E7DA-4475-A815-080F0E3DD429}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093F5732-F62A-4181-A2FD-49771FF0DAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="391">
   <si>
     <t>100nF</t>
   </si>
@@ -351,9 +351,6 @@
     <t>49.9Ω</t>
   </si>
   <si>
-    <t>C8475</t>
-  </si>
-  <si>
     <t>WJ301V-5.0-2P</t>
   </si>
   <si>
@@ -1126,6 +1123,78 @@
   </si>
   <si>
     <t xml:space="preserve">    L3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    C39</t>
+  </si>
+  <si>
+    <t>12pF</t>
+  </si>
+  <si>
+    <t>C1547</t>
+  </si>
+  <si>
+    <t>FH(Guangdong Fenghua Advanced Tech)</t>
+  </si>
+  <si>
+    <t>0402CG120J500NT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    C40</t>
+  </si>
+  <si>
+    <t>C8377</t>
+  </si>
+  <si>
+    <t>XY2500V-B-5.00-3P</t>
+  </si>
+  <si>
+    <t>C8445</t>
+  </si>
+  <si>
+    <t>C8446</t>
+  </si>
+  <si>
+    <t>XY2500V-B-5.00-4P</t>
+  </si>
+  <si>
+    <t>Ningbo Xinlaiya Elec.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    D20</t>
+  </si>
+  <si>
+    <t>C124383</t>
+  </si>
+  <si>
+    <t>Ckmtw(Shenzhen Cankemeng)</t>
+  </si>
+  <si>
+    <t>C126888</t>
+  </si>
+  <si>
+    <t>DSWB01LHGET</t>
+  </si>
+  <si>
+    <t>Dongguan Guangzhu Industrial</t>
+  </si>
+  <si>
+    <t>C158012</t>
+  </si>
+  <si>
+    <t>B2B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>JST Sales America</t>
+  </si>
+  <si>
+    <t>C473012</t>
+  </si>
+  <si>
+    <t>ESP32-WROOM-32D</t>
+  </si>
+  <si>
+    <t>Espressif Systems</t>
   </si>
 </sst>
 </file>
@@ -1508,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:G148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,13 +1610,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>200</v>
+        <v>179</v>
+      </c>
+      <c r="D2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" t="s">
+        <v>85</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1555,13 +1633,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>206</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>208</v>
+        <v>179</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" t="s">
+        <v>85</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1569,13 +1656,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>211</v>
+        <v>179</v>
+      </c>
+      <c r="D4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" t="s">
+        <v>85</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1583,13 +1679,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>212</v>
+        <v>179</v>
+      </c>
+      <c r="D5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" t="s">
+        <v>85</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1597,13 +1702,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>212</v>
+        <v>179</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" t="s">
+        <v>85</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -1611,13 +1725,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>179</v>
+      </c>
+      <c r="D7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1625,13 +1748,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="B8" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>212</v>
+        <v>179</v>
+      </c>
+      <c r="D8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" t="s">
+        <v>85</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1639,13 +1771,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>213</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>215</v>
+        <v>179</v>
+      </c>
+      <c r="D9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" t="s">
+        <v>85</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1653,19 +1794,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" t="s">
         <v>116</v>
-      </c>
-      <c r="E10" t="s">
-        <v>117</v>
       </c>
       <c r="F10" t="s">
         <v>85</v>
@@ -1676,19 +1817,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>216</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" t="s">
         <v>116</v>
-      </c>
-      <c r="E11" t="s">
-        <v>117</v>
       </c>
       <c r="F11" t="s">
         <v>85</v>
@@ -1699,19 +1840,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>217</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" t="s">
         <v>116</v>
-      </c>
-      <c r="E12" t="s">
-        <v>117</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
@@ -1722,19 +1863,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>218</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" t="s">
         <v>116</v>
-      </c>
-      <c r="E13" t="s">
-        <v>117</v>
       </c>
       <c r="F13" t="s">
         <v>85</v>
@@ -1745,19 +1886,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>219</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" t="s">
         <v>116</v>
-      </c>
-      <c r="E14" t="s">
-        <v>117</v>
       </c>
       <c r="F14" t="s">
         <v>85</v>
@@ -1768,19 +1909,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>220</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D15" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" t="s">
         <v>116</v>
-      </c>
-      <c r="E15" t="s">
-        <v>117</v>
       </c>
       <c r="F15" t="s">
         <v>85</v>
@@ -1791,19 +1932,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" t="s">
         <v>116</v>
-      </c>
-      <c r="E16" t="s">
-        <v>117</v>
       </c>
       <c r="F16" t="s">
         <v>85</v>
@@ -1814,19 +1955,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>222</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" t="s">
         <v>116</v>
-      </c>
-      <c r="E17" t="s">
-        <v>117</v>
       </c>
       <c r="F17" t="s">
         <v>85</v>
@@ -1837,19 +1978,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>223</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D18" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" t="s">
         <v>116</v>
-      </c>
-      <c r="E18" t="s">
-        <v>117</v>
       </c>
       <c r="F18" t="s">
         <v>85</v>
@@ -1860,19 +2001,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" t="s">
         <v>116</v>
-      </c>
-      <c r="E19" t="s">
-        <v>117</v>
       </c>
       <c r="F19" t="s">
         <v>85</v>
@@ -1883,22 +2024,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>218</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D20" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E20" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F20" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1906,22 +2047,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D21" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F21" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1929,22 +2070,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>220</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F22" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1952,22 +2093,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B23" t="s">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D23" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E23" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F23" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1975,22 +2116,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>222</v>
+        <v>367</v>
       </c>
       <c r="B24" t="s">
-        <v>0</v>
+        <v>368</v>
       </c>
       <c r="C24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D24" t="s">
-        <v>116</v>
+        <v>369</v>
       </c>
       <c r="E24" t="s">
-        <v>117</v>
+        <v>370</v>
       </c>
       <c r="F24" t="s">
-        <v>85</v>
+        <v>371</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -1998,22 +2139,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>223</v>
+        <v>372</v>
       </c>
       <c r="B25" t="s">
-        <v>0</v>
+        <v>368</v>
       </c>
       <c r="C25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D25" t="s">
-        <v>116</v>
+        <v>369</v>
       </c>
       <c r="E25" t="s">
-        <v>117</v>
+        <v>370</v>
       </c>
       <c r="F25" t="s">
-        <v>85</v>
+        <v>371</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -2021,22 +2162,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>224</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D26" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E26" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="F26" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -2044,22 +2185,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B27" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D27" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E27" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="F27" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -2067,22 +2208,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
         <v>180</v>
       </c>
       <c r="D28" t="s">
-        <v>118</v>
+        <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>119</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -2090,22 +2231,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>226</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
         <v>180</v>
       </c>
       <c r="D29" t="s">
-        <v>118</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>119</v>
+        <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -2113,22 +2254,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="E30" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="F30" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -2136,22 +2277,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D31" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="E31" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="F31" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -2159,22 +2300,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>229</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="C32" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E32" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="F32" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -2182,22 +2323,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="C33" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D33" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E33" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="F33" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -2205,22 +2346,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>231</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="C34" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>147</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>148</v>
       </c>
       <c r="F34" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -2228,22 +2369,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>232</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="C35" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D35" t="s">
-        <v>12</v>
+        <v>147</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
+        <v>148</v>
       </c>
       <c r="F35" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -2251,22 +2392,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>233</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>146</v>
       </c>
       <c r="C36" t="s">
         <v>182</v>
       </c>
       <c r="D36" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="E36" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="F36" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -2274,22 +2415,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>146</v>
       </c>
       <c r="C37" t="s">
         <v>182</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="E37" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="F37" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -2297,19 +2438,19 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" t="s">
+        <v>182</v>
+      </c>
+      <c r="D38" t="s">
         <v>147</v>
       </c>
-      <c r="C38" t="s">
-        <v>183</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>148</v>
-      </c>
-      <c r="E38" t="s">
-        <v>149</v>
       </c>
       <c r="F38" t="s">
         <v>15</v>
@@ -2320,19 +2461,19 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B39" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" t="s">
+        <v>182</v>
+      </c>
+      <c r="D39" t="s">
         <v>147</v>
       </c>
-      <c r="C39" t="s">
-        <v>183</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>148</v>
-      </c>
-      <c r="E39" t="s">
-        <v>149</v>
       </c>
       <c r="F39" t="s">
         <v>15</v>
@@ -2343,22 +2484,22 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>232</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>147</v>
+        <v>22</v>
       </c>
       <c r="C40" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D40" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
-        <v>149</v>
+        <v>22</v>
       </c>
       <c r="F40" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -2366,22 +2507,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>233</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>147</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D41" t="s">
-        <v>148</v>
+        <v>27</v>
       </c>
       <c r="E41" t="s">
-        <v>149</v>
+        <v>28</v>
       </c>
       <c r="F41" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -2389,22 +2530,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>234</v>
+        <v>166</v>
       </c>
       <c r="B42" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="C42" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="D42" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="E42" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="F42" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -2412,22 +2553,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="B43" t="s">
-        <v>147</v>
+        <v>241</v>
       </c>
       <c r="C43" t="s">
-        <v>183</v>
+        <v>242</v>
       </c>
       <c r="D43" t="s">
-        <v>148</v>
+        <v>373</v>
       </c>
       <c r="E43" t="s">
-        <v>149</v>
+        <v>374</v>
       </c>
       <c r="F43" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -2435,22 +2576,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>236</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="C44" t="s">
-        <v>183</v>
+        <v>237</v>
       </c>
       <c r="D44" t="s">
-        <v>148</v>
+        <v>375</v>
       </c>
       <c r="E44" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="F44" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -2458,22 +2599,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>238</v>
+      </c>
+      <c r="B45" t="s">
+        <v>239</v>
+      </c>
+      <c r="C45" t="s">
         <v>237</v>
       </c>
-      <c r="B45" t="s">
-        <v>147</v>
-      </c>
-      <c r="C45" t="s">
-        <v>183</v>
-      </c>
       <c r="D45" t="s">
-        <v>148</v>
+        <v>375</v>
       </c>
       <c r="E45" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="F45" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -2481,22 +2622,22 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>208</v>
       </c>
       <c r="B46" t="s">
-        <v>22</v>
+        <v>209</v>
       </c>
       <c r="C46" t="s">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="D46" t="s">
-        <v>23</v>
+        <v>376</v>
       </c>
       <c r="E46" t="s">
-        <v>22</v>
+        <v>377</v>
       </c>
       <c r="F46" t="s">
-        <v>24</v>
+        <v>378</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -2504,22 +2645,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>26</v>
+        <v>151</v>
       </c>
       <c r="C47" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D47" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="E47" t="s">
-        <v>28</v>
+        <v>151</v>
       </c>
       <c r="F47" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -2527,22 +2668,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B48" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="C48" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="D48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E48" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="F48" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -2550,22 +2691,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="B49" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="C49" t="s">
-        <v>238</v>
+        <v>180</v>
       </c>
       <c r="D49" t="s">
-        <v>109</v>
+        <v>165</v>
       </c>
       <c r="E49" t="s">
-        <v>110</v>
+        <v>151</v>
       </c>
       <c r="F49" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -2573,22 +2714,22 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>239</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>240</v>
+        <v>125</v>
       </c>
       <c r="C50" t="s">
-        <v>238</v>
+        <v>189</v>
       </c>
       <c r="D50" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="E50" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="F50" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -2596,22 +2737,22 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>241</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>242</v>
+        <v>125</v>
       </c>
       <c r="C51" t="s">
-        <v>243</v>
+        <v>189</v>
       </c>
       <c r="D51" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="E51" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="F51" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="G51">
         <v>1</v>
@@ -2619,19 +2760,19 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>151</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="C52" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D52" t="s">
-        <v>166</v>
+        <v>126</v>
       </c>
       <c r="E52" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="F52" t="s">
         <v>13</v>
@@ -2642,19 +2783,19 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>153</v>
+        <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="C53" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D53" t="s">
-        <v>166</v>
+        <v>126</v>
       </c>
       <c r="E53" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="F53" t="s">
         <v>13</v>
@@ -2665,19 +2806,19 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>243</v>
+      </c>
+      <c r="B54" t="s">
+        <v>125</v>
+      </c>
+      <c r="C54" t="s">
         <v>189</v>
       </c>
-      <c r="B54" t="s">
-        <v>152</v>
-      </c>
-      <c r="C54" t="s">
-        <v>181</v>
-      </c>
       <c r="D54" t="s">
-        <v>166</v>
+        <v>126</v>
       </c>
       <c r="E54" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="F54" t="s">
         <v>13</v>
@@ -2688,19 +2829,19 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>244</v>
       </c>
       <c r="B55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C55" t="s">
+        <v>189</v>
+      </c>
+      <c r="D55" t="s">
         <v>126</v>
       </c>
-      <c r="C55" t="s">
-        <v>190</v>
-      </c>
-      <c r="D55" t="s">
-        <v>127</v>
-      </c>
       <c r="E55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F55" t="s">
         <v>13</v>
@@ -2711,19 +2852,19 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>50</v>
+        <v>245</v>
       </c>
       <c r="B56" t="s">
+        <v>125</v>
+      </c>
+      <c r="C56" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" t="s">
         <v>126</v>
       </c>
-      <c r="C56" t="s">
-        <v>190</v>
-      </c>
-      <c r="D56" t="s">
-        <v>127</v>
-      </c>
       <c r="E56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F56" t="s">
         <v>13</v>
@@ -2734,19 +2875,19 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>246</v>
       </c>
       <c r="B57" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" t="s">
+        <v>189</v>
+      </c>
+      <c r="D57" t="s">
         <v>126</v>
       </c>
-      <c r="C57" t="s">
-        <v>190</v>
-      </c>
-      <c r="D57" t="s">
-        <v>127</v>
-      </c>
       <c r="E57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F57" t="s">
         <v>13</v>
@@ -2757,19 +2898,19 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>247</v>
       </c>
       <c r="B58" t="s">
+        <v>125</v>
+      </c>
+      <c r="C58" t="s">
+        <v>189</v>
+      </c>
+      <c r="D58" t="s">
         <v>126</v>
       </c>
-      <c r="C58" t="s">
-        <v>190</v>
-      </c>
-      <c r="D58" t="s">
-        <v>127</v>
-      </c>
       <c r="E58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F58" t="s">
         <v>13</v>
@@ -2780,19 +2921,19 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>244</v>
+        <v>379</v>
       </c>
       <c r="B59" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" t="s">
+        <v>189</v>
+      </c>
+      <c r="D59" t="s">
         <v>126</v>
       </c>
-      <c r="C59" t="s">
-        <v>190</v>
-      </c>
-      <c r="D59" t="s">
-        <v>127</v>
-      </c>
       <c r="E59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F59" t="s">
         <v>13</v>
@@ -2803,22 +2944,22 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>245</v>
+        <v>55</v>
       </c>
       <c r="B60" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
         <v>190</v>
       </c>
       <c r="D60" t="s">
-        <v>127</v>
+        <v>6</v>
       </c>
       <c r="E60" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="F60" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G60">
         <v>1</v>
@@ -2826,22 +2967,22 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>246</v>
+        <v>21</v>
       </c>
       <c r="B61" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C61" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D61" t="s">
+        <v>128</v>
+      </c>
+      <c r="E61" t="s">
         <v>127</v>
       </c>
-      <c r="E61" t="s">
-        <v>126</v>
-      </c>
       <c r="F61" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -2849,22 +2990,22 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>247</v>
+        <v>18</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="C62" t="s">
-        <v>190</v>
+        <v>248</v>
       </c>
       <c r="D62" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="E62" t="s">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="F62" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G62">
         <v>1</v>
@@ -2872,22 +3013,22 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>249</v>
+      </c>
+      <c r="B63" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" t="s">
         <v>248</v>
       </c>
-      <c r="B63" t="s">
-        <v>126</v>
-      </c>
-      <c r="C63" t="s">
-        <v>190</v>
-      </c>
       <c r="D63" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="E63" t="s">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="F63" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G63">
         <v>1</v>
@@ -2895,22 +3036,22 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>250</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>251</v>
       </c>
       <c r="C64" t="s">
         <v>191</v>
       </c>
       <c r="D64" t="s">
-        <v>6</v>
+        <v>252</v>
       </c>
       <c r="E64" t="s">
-        <v>5</v>
+        <v>253</v>
       </c>
       <c r="F64" t="s">
-        <v>7</v>
+        <v>254</v>
       </c>
       <c r="G64">
         <v>1</v>
@@ -2918,22 +3059,22 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="C65" t="s">
         <v>192</v>
       </c>
       <c r="D65" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="E65" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="F65" t="s">
-        <v>130</v>
+        <v>1</v>
       </c>
       <c r="G65">
         <v>1</v>
@@ -2941,22 +3082,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>18</v>
+        <v>255</v>
       </c>
       <c r="B66" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>249</v>
+        <v>192</v>
       </c>
       <c r="D66" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E66" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F66" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G66">
         <v>1</v>
@@ -2964,22 +3105,22 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>250</v>
+        <v>86</v>
       </c>
       <c r="B67" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C67" t="s">
-        <v>249</v>
+        <v>192</v>
       </c>
       <c r="D67" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E67" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F67" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G67">
         <v>1</v>
@@ -2987,22 +3128,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="B68" t="s">
-        <v>252</v>
+        <v>0</v>
       </c>
       <c r="C68" t="s">
-        <v>192</v>
+        <v>257</v>
       </c>
       <c r="D68" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="E68" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="F68" t="s">
-        <v>255</v>
+        <v>85</v>
       </c>
       <c r="G68">
         <v>1</v>
@@ -3010,19 +3151,19 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>38</v>
+        <v>260</v>
       </c>
       <c r="B69" t="s">
-        <v>82</v>
+        <v>261</v>
       </c>
       <c r="C69" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="D69" t="s">
-        <v>83</v>
+        <v>262</v>
       </c>
       <c r="E69" t="s">
-        <v>84</v>
+        <v>263</v>
       </c>
       <c r="F69" t="s">
         <v>1</v>
@@ -3033,19 +3174,19 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>261</v>
       </c>
       <c r="C70" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="D70" t="s">
-        <v>83</v>
+        <v>262</v>
       </c>
       <c r="E70" t="s">
-        <v>84</v>
+        <v>263</v>
       </c>
       <c r="F70" t="s">
         <v>1</v>
@@ -3056,22 +3197,22 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="B71" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="C71" t="s">
         <v>193</v>
       </c>
       <c r="D71" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
       <c r="E71" t="s">
-        <v>84</v>
+        <v>132</v>
       </c>
       <c r="F71" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G71">
         <v>1</v>
@@ -3079,22 +3220,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="B72" t="s">
-        <v>0</v>
+        <v>266</v>
       </c>
       <c r="C72" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="D72" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="E72" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="F72" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="G72">
         <v>1</v>
@@ -3102,22 +3243,22 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>261</v>
+        <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>262</v>
+        <v>16</v>
       </c>
       <c r="C73" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="D73" t="s">
-        <v>263</v>
+        <v>101</v>
       </c>
       <c r="E73" t="s">
-        <v>264</v>
+        <v>133</v>
       </c>
       <c r="F73" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G73">
         <v>1</v>
@@ -3125,22 +3266,22 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>265</v>
+        <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>262</v>
+        <v>16</v>
       </c>
       <c r="C74" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="D74" t="s">
-        <v>263</v>
+        <v>101</v>
       </c>
       <c r="E74" t="s">
-        <v>264</v>
+        <v>133</v>
       </c>
       <c r="F74" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G74">
         <v>1</v>
@@ -3148,16 +3289,16 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>131</v>
+        <v>16</v>
       </c>
       <c r="C75" t="s">
         <v>194</v>
       </c>
       <c r="D75" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="E75" t="s">
         <v>133</v>
@@ -3171,22 +3312,22 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>266</v>
+        <v>61</v>
       </c>
       <c r="B76" t="s">
-        <v>267</v>
+        <v>88</v>
       </c>
       <c r="C76" t="s">
-        <v>268</v>
+        <v>194</v>
       </c>
       <c r="D76" t="s">
-        <v>269</v>
+        <v>89</v>
       </c>
       <c r="E76" t="s">
-        <v>267</v>
+        <v>90</v>
       </c>
       <c r="F76" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G76">
         <v>1</v>
@@ -3194,19 +3335,19 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B77" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C77" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D77" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E77" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="F77" t="s">
         <v>15</v>
@@ -3217,19 +3358,19 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B78" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C78" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D78" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E78" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="F78" t="s">
         <v>15</v>
@@ -3240,19 +3381,19 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B79" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="C79" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D79" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E79" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="F79" t="s">
         <v>15</v>
@@ -3263,19 +3404,19 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>61</v>
+        <v>269</v>
       </c>
       <c r="B80" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="C80" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D80" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="E80" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="F80" t="s">
         <v>15</v>
@@ -3286,19 +3427,19 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>63</v>
+        <v>270</v>
       </c>
       <c r="B81" t="s">
-        <v>17</v>
+        <v>271</v>
       </c>
       <c r="C81" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="D81" t="s">
-        <v>102</v>
+        <v>272</v>
       </c>
       <c r="E81" t="s">
-        <v>103</v>
+        <v>273</v>
       </c>
       <c r="F81" t="s">
         <v>15</v>
@@ -3309,19 +3450,19 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B82" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C82" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="D82" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="E82" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="F82" t="s">
         <v>15</v>
@@ -3332,19 +3473,19 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B83" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="C83" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="D83" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="E83" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="F83" t="s">
         <v>15</v>
@@ -3355,19 +3496,19 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>270</v>
+        <v>154</v>
       </c>
       <c r="B84" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="C84" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="D84" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="E84" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="F84" t="s">
         <v>15</v>
@@ -3378,19 +3519,19 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>271</v>
+        <v>153</v>
       </c>
       <c r="B85" t="s">
-        <v>272</v>
+        <v>14</v>
       </c>
       <c r="C85" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D85" t="s">
-        <v>273</v>
+        <v>134</v>
       </c>
       <c r="E85" t="s">
-        <v>274</v>
+        <v>135</v>
       </c>
       <c r="F85" t="s">
         <v>15</v>
@@ -3401,19 +3542,19 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B86" t="s">
         <v>14</v>
       </c>
       <c r="C86" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D86" t="s">
+        <v>134</v>
+      </c>
+      <c r="E86" t="s">
         <v>135</v>
-      </c>
-      <c r="E86" t="s">
-        <v>136</v>
       </c>
       <c r="F86" t="s">
         <v>15</v>
@@ -3424,19 +3565,19 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B87" t="s">
         <v>14</v>
       </c>
       <c r="C87" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D87" t="s">
+        <v>134</v>
+      </c>
+      <c r="E87" t="s">
         <v>135</v>
-      </c>
-      <c r="E87" t="s">
-        <v>136</v>
       </c>
       <c r="F87" t="s">
         <v>15</v>
@@ -3453,13 +3594,13 @@
         <v>14</v>
       </c>
       <c r="C88" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D88" t="s">
+        <v>134</v>
+      </c>
+      <c r="E88" t="s">
         <v>135</v>
-      </c>
-      <c r="E88" t="s">
-        <v>136</v>
       </c>
       <c r="F88" t="s">
         <v>15</v>
@@ -3470,19 +3611,19 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B89" t="s">
         <v>14</v>
       </c>
       <c r="C89" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D89" t="s">
+        <v>134</v>
+      </c>
+      <c r="E89" t="s">
         <v>135</v>
-      </c>
-      <c r="E89" t="s">
-        <v>136</v>
       </c>
       <c r="F89" t="s">
         <v>15</v>
@@ -3493,19 +3634,19 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>70</v>
+        <v>157</v>
       </c>
       <c r="B90" t="s">
         <v>14</v>
       </c>
       <c r="C90" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D90" t="s">
+        <v>134</v>
+      </c>
+      <c r="E90" t="s">
         <v>135</v>
-      </c>
-      <c r="E90" t="s">
-        <v>136</v>
       </c>
       <c r="F90" t="s">
         <v>15</v>
@@ -3516,19 +3657,19 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="B91" t="s">
         <v>14</v>
       </c>
       <c r="C91" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D91" t="s">
+        <v>134</v>
+      </c>
+      <c r="E91" t="s">
         <v>135</v>
-      </c>
-      <c r="E91" t="s">
-        <v>136</v>
       </c>
       <c r="F91" t="s">
         <v>15</v>
@@ -3539,19 +3680,19 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>156</v>
+        <v>72</v>
       </c>
       <c r="B92" t="s">
         <v>14</v>
       </c>
       <c r="C92" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D92" t="s">
+        <v>134</v>
+      </c>
+      <c r="E92" t="s">
         <v>135</v>
-      </c>
-      <c r="E92" t="s">
-        <v>136</v>
       </c>
       <c r="F92" t="s">
         <v>15</v>
@@ -3562,19 +3703,19 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>157</v>
+        <v>73</v>
       </c>
       <c r="B93" t="s">
         <v>14</v>
       </c>
       <c r="C93" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D93" t="s">
+        <v>134</v>
+      </c>
+      <c r="E93" t="s">
         <v>135</v>
-      </c>
-      <c r="E93" t="s">
-        <v>136</v>
       </c>
       <c r="F93" t="s">
         <v>15</v>
@@ -3585,19 +3726,19 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>158</v>
+        <v>75</v>
       </c>
       <c r="B94" t="s">
         <v>14</v>
       </c>
       <c r="C94" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D94" t="s">
+        <v>134</v>
+      </c>
+      <c r="E94" t="s">
         <v>135</v>
-      </c>
-      <c r="E94" t="s">
-        <v>136</v>
       </c>
       <c r="F94" t="s">
         <v>15</v>
@@ -3614,13 +3755,13 @@
         <v>14</v>
       </c>
       <c r="C95" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D95" t="s">
+        <v>134</v>
+      </c>
+      <c r="E95" t="s">
         <v>135</v>
-      </c>
-      <c r="E95" t="s">
-        <v>136</v>
       </c>
       <c r="F95" t="s">
         <v>15</v>
@@ -3631,19 +3772,19 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="B96" t="s">
         <v>14</v>
       </c>
       <c r="C96" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D96" t="s">
+        <v>134</v>
+      </c>
+      <c r="E96" t="s">
         <v>135</v>
-      </c>
-      <c r="E96" t="s">
-        <v>136</v>
       </c>
       <c r="F96" t="s">
         <v>15</v>
@@ -3654,19 +3795,19 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>73</v>
+        <v>198</v>
       </c>
       <c r="B97" t="s">
         <v>14</v>
       </c>
       <c r="C97" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D97" t="s">
+        <v>134</v>
+      </c>
+      <c r="E97" t="s">
         <v>135</v>
-      </c>
-      <c r="E97" t="s">
-        <v>136</v>
       </c>
       <c r="F97" t="s">
         <v>15</v>
@@ -3677,19 +3818,19 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>75</v>
+        <v>195</v>
       </c>
       <c r="B98" t="s">
         <v>14</v>
       </c>
       <c r="C98" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D98" t="s">
+        <v>134</v>
+      </c>
+      <c r="E98" t="s">
         <v>135</v>
-      </c>
-      <c r="E98" t="s">
-        <v>136</v>
       </c>
       <c r="F98" t="s">
         <v>15</v>
@@ -3700,19 +3841,19 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>160</v>
+        <v>274</v>
       </c>
       <c r="B99" t="s">
         <v>14</v>
       </c>
       <c r="C99" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D99" t="s">
+        <v>134</v>
+      </c>
+      <c r="E99" t="s">
         <v>135</v>
-      </c>
-      <c r="E99" t="s">
-        <v>136</v>
       </c>
       <c r="F99" t="s">
         <v>15</v>
@@ -3723,19 +3864,19 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>161</v>
+        <v>275</v>
       </c>
       <c r="B100" t="s">
         <v>14</v>
       </c>
       <c r="C100" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D100" t="s">
+        <v>134</v>
+      </c>
+      <c r="E100" t="s">
         <v>135</v>
-      </c>
-      <c r="E100" t="s">
-        <v>136</v>
       </c>
       <c r="F100" t="s">
         <v>15</v>
@@ -3746,19 +3887,19 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>199</v>
+        <v>276</v>
       </c>
       <c r="B101" t="s">
         <v>14</v>
       </c>
       <c r="C101" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D101" t="s">
+        <v>134</v>
+      </c>
+      <c r="E101" t="s">
         <v>135</v>
-      </c>
-      <c r="E101" t="s">
-        <v>136</v>
       </c>
       <c r="F101" t="s">
         <v>15</v>
@@ -3769,19 +3910,19 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>196</v>
+        <v>277</v>
       </c>
       <c r="B102" t="s">
-        <v>14</v>
+        <v>278</v>
       </c>
       <c r="C102" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D102" t="s">
-        <v>135</v>
+        <v>279</v>
       </c>
       <c r="E102" t="s">
-        <v>136</v>
+        <v>280</v>
       </c>
       <c r="F102" t="s">
         <v>15</v>
@@ -3792,19 +3933,19 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>275</v>
+        <v>145</v>
       </c>
       <c r="B103" t="s">
-        <v>14</v>
+        <v>281</v>
       </c>
       <c r="C103" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D103" t="s">
-        <v>135</v>
+        <v>282</v>
       </c>
       <c r="E103" t="s">
-        <v>136</v>
+        <v>283</v>
       </c>
       <c r="F103" t="s">
         <v>15</v>
@@ -3815,19 +3956,19 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>276</v>
+        <v>183</v>
       </c>
       <c r="B104" t="s">
-        <v>14</v>
+        <v>281</v>
       </c>
       <c r="C104" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D104" t="s">
-        <v>135</v>
+        <v>282</v>
       </c>
       <c r="E104" t="s">
-        <v>136</v>
+        <v>283</v>
       </c>
       <c r="F104" t="s">
         <v>15</v>
@@ -3838,19 +3979,19 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>277</v>
+        <v>184</v>
       </c>
       <c r="B105" t="s">
-        <v>14</v>
+        <v>281</v>
       </c>
       <c r="C105" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D105" t="s">
-        <v>135</v>
+        <v>282</v>
       </c>
       <c r="E105" t="s">
-        <v>136</v>
+        <v>283</v>
       </c>
       <c r="F105" t="s">
         <v>15</v>
@@ -3861,19 +4002,19 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>278</v>
+        <v>185</v>
       </c>
       <c r="B106" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C106" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D106" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E106" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="F106" t="s">
         <v>15</v>
@@ -3884,19 +4025,19 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>146</v>
+        <v>284</v>
       </c>
       <c r="B107" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C107" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D107" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E107" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="F107" t="s">
         <v>15</v>
@@ -3907,19 +4048,19 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>184</v>
+        <v>288</v>
       </c>
       <c r="B108" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="C108" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D108" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="E108" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="F108" t="s">
         <v>15</v>
@@ -3930,19 +4071,19 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>185</v>
+        <v>292</v>
       </c>
       <c r="B109" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="C109" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D109" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="E109" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="F109" t="s">
         <v>15</v>
@@ -3953,19 +4094,19 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>186</v>
+        <v>149</v>
       </c>
       <c r="B110" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="C110" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="D110" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
       <c r="E110" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="F110" t="s">
         <v>15</v>
@@ -3976,19 +4117,19 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>285</v>
+        <v>76</v>
       </c>
       <c r="B111" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="C111" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="D111" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="E111" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="F111" t="s">
         <v>15</v>
@@ -3999,19 +4140,19 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>289</v>
+        <v>197</v>
       </c>
       <c r="B112" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C112" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="D112" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="E112" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="F112" t="s">
         <v>15</v>
@@ -4022,19 +4163,19 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>293</v>
+        <v>196</v>
       </c>
       <c r="B113" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C113" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="D113" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E113" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="F113" t="s">
         <v>15</v>
@@ -4045,19 +4186,19 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>150</v>
+        <v>68</v>
       </c>
       <c r="B114" t="s">
-        <v>297</v>
+        <v>91</v>
       </c>
       <c r="C114" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D114" t="s">
-        <v>298</v>
+        <v>136</v>
       </c>
       <c r="E114" t="s">
-        <v>299</v>
+        <v>137</v>
       </c>
       <c r="F114" t="s">
         <v>15</v>
@@ -4068,19 +4209,19 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>76</v>
+        <v>299</v>
       </c>
       <c r="B115" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C115" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D115" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="E115" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="F115" t="s">
         <v>15</v>
@@ -4091,22 +4232,22 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>198</v>
+        <v>303</v>
       </c>
       <c r="B116" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="C116" t="s">
-        <v>194</v>
+        <v>305</v>
       </c>
       <c r="D116" t="s">
-        <v>298</v>
+        <v>176</v>
       </c>
       <c r="E116" t="s">
-        <v>299</v>
+        <v>177</v>
       </c>
       <c r="F116" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
       <c r="G116">
         <v>1</v>
@@ -4114,22 +4255,22 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>197</v>
+        <v>306</v>
       </c>
       <c r="B117" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="C117" t="s">
-        <v>194</v>
+        <v>308</v>
       </c>
       <c r="D117" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="E117" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="F117" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G117">
         <v>1</v>
@@ -4137,22 +4278,22 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>68</v>
+        <v>311</v>
       </c>
       <c r="B118" t="s">
-        <v>91</v>
+        <v>312</v>
       </c>
       <c r="C118" t="s">
-        <v>183</v>
+        <v>267</v>
       </c>
       <c r="D118" t="s">
-        <v>137</v>
+        <v>313</v>
       </c>
       <c r="E118" t="s">
-        <v>138</v>
+        <v>314</v>
       </c>
       <c r="F118" t="s">
-        <v>15</v>
+        <v>315</v>
       </c>
       <c r="G118">
         <v>1</v>
@@ -4160,22 +4301,22 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>300</v>
+        <v>316</v>
       </c>
       <c r="B119" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
       <c r="C119" t="s">
-        <v>183</v>
+        <v>267</v>
       </c>
       <c r="D119" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="E119" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="F119" t="s">
-        <v>15</v>
+        <v>315</v>
       </c>
       <c r="G119">
         <v>1</v>
@@ -4183,22 +4324,22 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="B120" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="C120" t="s">
-        <v>306</v>
+        <v>267</v>
       </c>
       <c r="D120" t="s">
-        <v>177</v>
+        <v>313</v>
       </c>
       <c r="E120" t="s">
-        <v>178</v>
+        <v>314</v>
       </c>
       <c r="F120" t="s">
-        <v>179</v>
+        <v>315</v>
       </c>
       <c r="G120">
         <v>1</v>
@@ -4206,22 +4347,22 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="B121" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C121" t="s">
-        <v>309</v>
+        <v>267</v>
       </c>
       <c r="D121" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="E121" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="F121" t="s">
-        <v>20</v>
+        <v>315</v>
       </c>
       <c r="G121">
         <v>1</v>
@@ -4229,22 +4370,22 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="B122" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C122" t="s">
-        <v>268</v>
+        <v>179</v>
       </c>
       <c r="D122" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="E122" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="F122" t="s">
-        <v>316</v>
+        <v>1</v>
       </c>
       <c r="G122">
         <v>1</v>
@@ -4252,22 +4393,22 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="B123" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C123" t="s">
-        <v>268</v>
+        <v>179</v>
       </c>
       <c r="D123" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="E123" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="F123" t="s">
-        <v>316</v>
+        <v>1</v>
       </c>
       <c r="G123">
         <v>1</v>
@@ -4275,22 +4416,22 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>318</v>
+        <v>171</v>
       </c>
       <c r="B124" t="s">
-        <v>313</v>
+        <v>172</v>
       </c>
       <c r="C124" t="s">
-        <v>268</v>
+        <v>173</v>
       </c>
       <c r="D124" t="s">
-        <v>314</v>
+        <v>174</v>
       </c>
       <c r="E124" t="s">
-        <v>315</v>
+        <v>172</v>
       </c>
       <c r="F124" t="s">
-        <v>316</v>
+        <v>175</v>
       </c>
       <c r="G124">
         <v>1</v>
@@ -4298,22 +4439,22 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>319</v>
+        <v>52</v>
       </c>
       <c r="B125" t="s">
-        <v>313</v>
+        <v>8</v>
       </c>
       <c r="C125" t="s">
-        <v>268</v>
+        <v>181</v>
       </c>
       <c r="D125" t="s">
-        <v>314</v>
+        <v>106</v>
       </c>
       <c r="E125" t="s">
-        <v>315</v>
+        <v>107</v>
       </c>
       <c r="F125" t="s">
-        <v>316</v>
+        <v>100</v>
       </c>
       <c r="G125">
         <v>1</v>
@@ -4321,19 +4462,19 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>320</v>
+        <v>39</v>
       </c>
       <c r="B126" t="s">
-        <v>321</v>
+        <v>93</v>
       </c>
       <c r="C126" t="s">
-        <v>180</v>
+        <v>324</v>
       </c>
       <c r="D126" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="E126" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F126" t="s">
         <v>1</v>
@@ -4344,19 +4485,19 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>40</v>
+      </c>
+      <c r="B127" t="s">
+        <v>93</v>
+      </c>
+      <c r="C127" t="s">
         <v>324</v>
       </c>
-      <c r="B127" t="s">
-        <v>321</v>
-      </c>
-      <c r="C127" t="s">
-        <v>180</v>
-      </c>
       <c r="D127" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="E127" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F127" t="s">
         <v>1</v>
@@ -4367,22 +4508,22 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>172</v>
+        <v>327</v>
       </c>
       <c r="B128" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="C128" t="s">
-        <v>174</v>
+        <v>328</v>
       </c>
       <c r="D128" t="s">
-        <v>175</v>
+        <v>329</v>
       </c>
       <c r="E128" t="s">
-        <v>173</v>
+        <v>330</v>
       </c>
       <c r="F128" t="s">
-        <v>176</v>
+        <v>331</v>
       </c>
       <c r="G128">
         <v>1</v>
@@ -4390,22 +4531,22 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>52</v>
+        <v>332</v>
       </c>
       <c r="B129" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="C129" t="s">
-        <v>182</v>
+        <v>328</v>
       </c>
       <c r="D129" t="s">
-        <v>106</v>
+        <v>329</v>
       </c>
       <c r="E129" t="s">
-        <v>107</v>
+        <v>330</v>
       </c>
       <c r="F129" t="s">
-        <v>100</v>
+        <v>331</v>
       </c>
       <c r="G129">
         <v>1</v>
@@ -4413,22 +4554,22 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>39</v>
+        <v>333</v>
       </c>
       <c r="B130" t="s">
-        <v>93</v>
+        <v>334</v>
       </c>
       <c r="C130" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="D130" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="E130" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="F130" t="s">
-        <v>1</v>
+        <v>331</v>
       </c>
       <c r="G130">
         <v>1</v>
@@ -4436,22 +4577,22 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B131" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C131" t="s">
-        <v>325</v>
+        <v>112</v>
       </c>
       <c r="D131" t="s">
-        <v>326</v>
+        <v>113</v>
       </c>
       <c r="E131" t="s">
-        <v>327</v>
+        <v>111</v>
       </c>
       <c r="F131" t="s">
-        <v>1</v>
+        <v>114</v>
       </c>
       <c r="G131">
         <v>1</v>
@@ -4459,22 +4600,22 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>328</v>
+        <v>43</v>
       </c>
       <c r="B132" t="s">
         <v>93</v>
       </c>
       <c r="C132" t="s">
-        <v>329</v>
+        <v>192</v>
       </c>
       <c r="D132" t="s">
-        <v>330</v>
+        <v>94</v>
       </c>
       <c r="E132" t="s">
-        <v>331</v>
+        <v>95</v>
       </c>
       <c r="F132" t="s">
-        <v>332</v>
+        <v>1</v>
       </c>
       <c r="G132">
         <v>1</v>
@@ -4482,22 +4623,22 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>333</v>
+        <v>44</v>
       </c>
       <c r="B133" t="s">
         <v>93</v>
       </c>
       <c r="C133" t="s">
-        <v>329</v>
+        <v>192</v>
       </c>
       <c r="D133" t="s">
-        <v>330</v>
+        <v>94</v>
       </c>
       <c r="E133" t="s">
-        <v>331</v>
+        <v>95</v>
       </c>
       <c r="F133" t="s">
-        <v>332</v>
+        <v>1</v>
       </c>
       <c r="G133">
         <v>1</v>
@@ -4505,22 +4646,22 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="B134" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C134" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D134" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="E134" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="F134" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="G134">
         <v>1</v>
@@ -4528,22 +4669,22 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>53</v>
+        <v>205</v>
       </c>
       <c r="B135" t="s">
-        <v>112</v>
+        <v>206</v>
       </c>
       <c r="C135" t="s">
-        <v>113</v>
+        <v>207</v>
       </c>
       <c r="D135" t="s">
-        <v>114</v>
+        <v>380</v>
       </c>
       <c r="E135" t="s">
-        <v>112</v>
+        <v>380</v>
       </c>
       <c r="F135" t="s">
-        <v>115</v>
+        <v>381</v>
       </c>
       <c r="G135">
         <v>1</v>
@@ -4551,22 +4692,22 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="B136" t="s">
-        <v>93</v>
+        <v>200</v>
       </c>
       <c r="C136" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="D136" t="s">
-        <v>94</v>
+        <v>382</v>
       </c>
       <c r="E136" t="s">
-        <v>95</v>
+        <v>383</v>
       </c>
       <c r="F136" t="s">
-        <v>1</v>
+        <v>384</v>
       </c>
       <c r="G136">
         <v>1</v>
@@ -4574,22 +4715,22 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>44</v>
+        <v>162</v>
       </c>
       <c r="B137" t="s">
-        <v>93</v>
+        <v>200</v>
       </c>
       <c r="C137" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="D137" t="s">
-        <v>94</v>
+        <v>382</v>
       </c>
       <c r="E137" t="s">
-        <v>95</v>
+        <v>383</v>
       </c>
       <c r="F137" t="s">
-        <v>1</v>
+        <v>384</v>
       </c>
       <c r="G137">
         <v>1</v>
@@ -4597,22 +4738,22 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>339</v>
+        <v>201</v>
       </c>
       <c r="B138" t="s">
-        <v>340</v>
+        <v>200</v>
       </c>
       <c r="C138" t="s">
-        <v>341</v>
+        <v>211</v>
       </c>
       <c r="D138" t="s">
-        <v>342</v>
+        <v>382</v>
       </c>
       <c r="E138" t="s">
-        <v>343</v>
+        <v>383</v>
       </c>
       <c r="F138" t="s">
-        <v>344</v>
+        <v>384</v>
       </c>
       <c r="G138">
         <v>1</v>
@@ -4620,22 +4761,22 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>345</v>
+        <v>202</v>
       </c>
       <c r="B139" t="s">
-        <v>346</v>
+        <v>200</v>
       </c>
       <c r="C139" t="s">
-        <v>347</v>
+        <v>211</v>
       </c>
       <c r="D139" t="s">
-        <v>348</v>
+        <v>382</v>
       </c>
       <c r="E139" t="s">
-        <v>349</v>
+        <v>383</v>
       </c>
       <c r="F139" t="s">
-        <v>350</v>
+        <v>384</v>
       </c>
       <c r="G139">
         <v>1</v>
@@ -4643,22 +4784,22 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="B140" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="C140" t="s">
+        <v>346</v>
+      </c>
+      <c r="D140" t="s">
         <v>347</v>
       </c>
-      <c r="D140" t="s">
-        <v>353</v>
-      </c>
       <c r="E140" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F140" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="G140">
         <v>1</v>
@@ -4666,22 +4807,22 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>355</v>
+        <v>203</v>
       </c>
       <c r="B141" t="s">
-        <v>356</v>
+        <v>204</v>
       </c>
       <c r="C141" t="s">
-        <v>357</v>
+        <v>199</v>
       </c>
       <c r="D141" t="s">
-        <v>358</v>
+        <v>385</v>
       </c>
       <c r="E141" t="s">
-        <v>359</v>
+        <v>386</v>
       </c>
       <c r="F141" t="s">
-        <v>360</v>
+        <v>387</v>
       </c>
       <c r="G141">
         <v>1</v>
@@ -4689,22 +4830,22 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="B142" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="C142" t="s">
-        <v>363</v>
+        <v>346</v>
       </c>
       <c r="D142" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="E142" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="F142" t="s">
-        <v>20</v>
+        <v>353</v>
       </c>
       <c r="G142">
         <v>1</v>
@@ -4712,22 +4853,22 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>139</v>
+        <v>354</v>
       </c>
       <c r="B143" t="s">
-        <v>140</v>
+        <v>355</v>
       </c>
       <c r="C143" t="s">
-        <v>141</v>
+        <v>356</v>
       </c>
       <c r="D143" t="s">
-        <v>142</v>
+        <v>357</v>
       </c>
       <c r="E143" t="s">
-        <v>143</v>
+        <v>358</v>
       </c>
       <c r="F143" t="s">
-        <v>144</v>
+        <v>359</v>
       </c>
       <c r="G143">
         <v>1</v>
@@ -4735,22 +4876,22 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>58</v>
+        <v>360</v>
       </c>
       <c r="B144" t="s">
-        <v>9</v>
+        <v>361</v>
       </c>
       <c r="C144" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D144" t="s">
-        <v>164</v>
+        <v>363</v>
       </c>
       <c r="E144" t="s">
-        <v>165</v>
+        <v>364</v>
       </c>
       <c r="F144" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G144">
         <v>1</v>
@@ -4758,24 +4899,93 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>367</v>
+        <v>138</v>
       </c>
       <c r="B145" t="s">
+        <v>139</v>
+      </c>
+      <c r="C145" t="s">
+        <v>140</v>
+      </c>
+      <c r="D145" t="s">
+        <v>141</v>
+      </c>
+      <c r="E145" t="s">
+        <v>142</v>
+      </c>
+      <c r="F145" t="s">
+        <v>143</v>
+      </c>
+      <c r="G145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>58</v>
+      </c>
+      <c r="B146" t="s">
         <v>9</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C146" t="s">
+        <v>365</v>
+      </c>
+      <c r="D146" t="s">
+        <v>163</v>
+      </c>
+      <c r="E146" t="s">
+        <v>164</v>
+      </c>
+      <c r="F146" t="s">
+        <v>10</v>
+      </c>
+      <c r="G146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>366</v>
       </c>
-      <c r="D145" t="s">
+      <c r="B147" t="s">
+        <v>9</v>
+      </c>
+      <c r="C147" t="s">
+        <v>365</v>
+      </c>
+      <c r="D147" t="s">
+        <v>163</v>
+      </c>
+      <c r="E147" t="s">
         <v>164</v>
       </c>
-      <c r="E145" t="s">
-        <v>165</v>
-      </c>
-      <c r="F145" t="s">
+      <c r="F147" t="s">
         <v>10</v>
       </c>
-      <c r="G145">
+      <c r="G147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>212</v>
+      </c>
+      <c r="B148" t="s">
+        <v>213</v>
+      </c>
+      <c r="C148" t="s">
+        <v>214</v>
+      </c>
+      <c r="D148" t="s">
+        <v>388</v>
+      </c>
+      <c r="E148" t="s">
+        <v>389</v>
+      </c>
+      <c r="F148" t="s">
+        <v>390</v>
+      </c>
+      <c r="G148">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
temperature on board tested
</commit_message>
<xml_diff>
--- a/AnthC-M1R1/BOM esp32 Core  V-0.1.xlsx
+++ b/AnthC-M1R1/BOM esp32 Core  V-0.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doen_\Documents\Working\Anthilla\esp32 Core  V-0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093F5732-F62A-4181-A2FD-49771FF0DAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95CE96B-1F21-4A9E-B094-5160588008A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="392">
   <si>
     <t>100nF</t>
   </si>
@@ -1195,6 +1195,9 @@
   </si>
   <si>
     <t>Espressif Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    C41</t>
   </si>
 </sst>
 </file>
@@ -1577,10 +1580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G148"/>
+  <dimension ref="A1:G149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3197,22 +3200,22 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>391</v>
       </c>
       <c r="B71" t="s">
-        <v>130</v>
+        <v>261</v>
       </c>
       <c r="C71" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="D71" t="s">
-        <v>131</v>
+        <v>262</v>
       </c>
       <c r="E71" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="F71" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G71">
         <v>1</v>
@@ -3220,22 +3223,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>265</v>
+        <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>266</v>
+        <v>130</v>
       </c>
       <c r="C72" t="s">
-        <v>267</v>
+        <v>193</v>
       </c>
       <c r="D72" t="s">
-        <v>268</v>
+        <v>131</v>
       </c>
       <c r="E72" t="s">
-        <v>266</v>
+        <v>132</v>
       </c>
       <c r="F72" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G72">
         <v>1</v>
@@ -3243,22 +3246,22 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>66</v>
+        <v>265</v>
       </c>
       <c r="B73" t="s">
-        <v>16</v>
+        <v>266</v>
       </c>
       <c r="C73" t="s">
-        <v>194</v>
+        <v>267</v>
       </c>
       <c r="D73" t="s">
-        <v>101</v>
+        <v>268</v>
       </c>
       <c r="E73" t="s">
-        <v>133</v>
+        <v>266</v>
       </c>
       <c r="F73" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G73">
         <v>1</v>
@@ -3266,7 +3269,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B74" t="s">
         <v>16</v>
@@ -3289,7 +3292,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>16</v>
@@ -3312,19 +3315,19 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="C76" t="s">
         <v>194</v>
       </c>
       <c r="D76" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="E76" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
       <c r="F76" t="s">
         <v>15</v>
@@ -3335,19 +3338,19 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="C77" t="s">
         <v>194</v>
       </c>
       <c r="D77" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E77" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="F77" t="s">
         <v>15</v>
@@ -3358,7 +3361,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B78" t="s">
         <v>17</v>
@@ -3381,19 +3384,19 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B79" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="C79" t="s">
         <v>194</v>
       </c>
       <c r="D79" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E79" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F79" t="s">
         <v>15</v>
@@ -3404,7 +3407,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>269</v>
+        <v>62</v>
       </c>
       <c r="B80" t="s">
         <v>108</v>
@@ -3427,19 +3430,19 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B81" t="s">
-        <v>271</v>
+        <v>108</v>
       </c>
       <c r="C81" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="D81" t="s">
-        <v>272</v>
+        <v>104</v>
       </c>
       <c r="E81" t="s">
-        <v>273</v>
+        <v>105</v>
       </c>
       <c r="F81" t="s">
         <v>15</v>
@@ -3450,19 +3453,19 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>67</v>
+        <v>270</v>
       </c>
       <c r="B82" t="s">
-        <v>14</v>
+        <v>271</v>
       </c>
       <c r="C82" t="s">
         <v>182</v>
       </c>
       <c r="D82" t="s">
-        <v>134</v>
+        <v>272</v>
       </c>
       <c r="E82" t="s">
-        <v>135</v>
+        <v>273</v>
       </c>
       <c r="F82" t="s">
         <v>15</v>
@@ -3473,7 +3476,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B83" t="s">
         <v>14</v>
@@ -3496,7 +3499,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>154</v>
+        <v>69</v>
       </c>
       <c r="B84" t="s">
         <v>14</v>
@@ -3519,7 +3522,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B85" t="s">
         <v>14</v>
@@ -3542,7 +3545,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>70</v>
+        <v>153</v>
       </c>
       <c r="B86" t="s">
         <v>14</v>
@@ -3565,7 +3568,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B87" t="s">
         <v>14</v>
@@ -3588,7 +3591,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>155</v>
+        <v>71</v>
       </c>
       <c r="B88" t="s">
         <v>14</v>
@@ -3611,7 +3614,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B89" t="s">
         <v>14</v>
@@ -3634,7 +3637,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B90" t="s">
         <v>14</v>
@@ -3657,7 +3660,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B91" t="s">
         <v>14</v>
@@ -3680,7 +3683,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>72</v>
+        <v>158</v>
       </c>
       <c r="B92" t="s">
         <v>14</v>
@@ -3703,7 +3706,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B93" t="s">
         <v>14</v>
@@ -3726,7 +3729,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B94" t="s">
         <v>14</v>
@@ -3749,7 +3752,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>159</v>
+        <v>75</v>
       </c>
       <c r="B95" t="s">
         <v>14</v>
@@ -3772,7 +3775,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B96" t="s">
         <v>14</v>
@@ -3795,7 +3798,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="B97" t="s">
         <v>14</v>
@@ -3818,7 +3821,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B98" t="s">
         <v>14</v>
@@ -3841,7 +3844,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>274</v>
+        <v>195</v>
       </c>
       <c r="B99" t="s">
         <v>14</v>
@@ -3864,7 +3867,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B100" t="s">
         <v>14</v>
@@ -3887,7 +3890,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B101" t="s">
         <v>14</v>
@@ -3910,19 +3913,19 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B102" t="s">
-        <v>278</v>
+        <v>14</v>
       </c>
       <c r="C102" t="s">
         <v>182</v>
       </c>
       <c r="D102" t="s">
-        <v>279</v>
+        <v>134</v>
       </c>
       <c r="E102" t="s">
-        <v>280</v>
+        <v>135</v>
       </c>
       <c r="F102" t="s">
         <v>15</v>
@@ -3933,19 +3936,19 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>145</v>
+        <v>277</v>
       </c>
       <c r="B103" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C103" t="s">
         <v>182</v>
       </c>
       <c r="D103" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E103" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F103" t="s">
         <v>15</v>
@@ -3956,7 +3959,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>183</v>
+        <v>145</v>
       </c>
       <c r="B104" t="s">
         <v>281</v>
@@ -3979,7 +3982,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B105" t="s">
         <v>281</v>
@@ -4002,7 +4005,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B106" t="s">
         <v>281</v>
@@ -4025,19 +4028,19 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>284</v>
+        <v>185</v>
       </c>
       <c r="B107" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C107" t="s">
         <v>182</v>
       </c>
       <c r="D107" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E107" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F107" t="s">
         <v>15</v>
@@ -4048,19 +4051,19 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B108" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C108" t="s">
         <v>182</v>
       </c>
       <c r="D108" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E108" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F108" t="s">
         <v>15</v>
@@ -4071,19 +4074,19 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B109" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C109" t="s">
         <v>182</v>
       </c>
       <c r="D109" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E109" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F109" t="s">
         <v>15</v>
@@ -4094,19 +4097,19 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>149</v>
+        <v>292</v>
       </c>
       <c r="B110" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C110" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D110" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E110" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F110" t="s">
         <v>15</v>
@@ -4117,7 +4120,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>76</v>
+        <v>149</v>
       </c>
       <c r="B111" t="s">
         <v>296</v>
@@ -4140,7 +4143,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>197</v>
+        <v>76</v>
       </c>
       <c r="B112" t="s">
         <v>296</v>
@@ -4163,7 +4166,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B113" t="s">
         <v>296</v>
@@ -4186,19 +4189,19 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>68</v>
+        <v>196</v>
       </c>
       <c r="B114" t="s">
-        <v>91</v>
+        <v>296</v>
       </c>
       <c r="C114" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="D114" t="s">
-        <v>136</v>
+        <v>297</v>
       </c>
       <c r="E114" t="s">
-        <v>137</v>
+        <v>298</v>
       </c>
       <c r="F114" t="s">
         <v>15</v>
@@ -4209,19 +4212,19 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>299</v>
+        <v>68</v>
       </c>
       <c r="B115" t="s">
-        <v>300</v>
+        <v>91</v>
       </c>
       <c r="C115" t="s">
         <v>182</v>
       </c>
       <c r="D115" t="s">
-        <v>301</v>
+        <v>136</v>
       </c>
       <c r="E115" t="s">
-        <v>302</v>
+        <v>137</v>
       </c>
       <c r="F115" t="s">
         <v>15</v>
@@ -4232,22 +4235,22 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B116" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C116" t="s">
-        <v>305</v>
+        <v>182</v>
       </c>
       <c r="D116" t="s">
-        <v>176</v>
+        <v>301</v>
       </c>
       <c r="E116" t="s">
-        <v>177</v>
+        <v>302</v>
       </c>
       <c r="F116" t="s">
-        <v>178</v>
+        <v>15</v>
       </c>
       <c r="G116">
         <v>1</v>
@@ -4255,22 +4258,22 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B117" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C117" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D117" t="s">
-        <v>309</v>
+        <v>176</v>
       </c>
       <c r="E117" t="s">
-        <v>310</v>
+        <v>177</v>
       </c>
       <c r="F117" t="s">
-        <v>20</v>
+        <v>178</v>
       </c>
       <c r="G117">
         <v>1</v>
@@ -4278,22 +4281,22 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B118" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C118" t="s">
-        <v>267</v>
+        <v>308</v>
       </c>
       <c r="D118" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E118" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F118" t="s">
-        <v>315</v>
+        <v>20</v>
       </c>
       <c r="G118">
         <v>1</v>
@@ -4301,7 +4304,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B119" t="s">
         <v>312</v>
@@ -4324,7 +4327,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B120" t="s">
         <v>312</v>
@@ -4347,7 +4350,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B121" t="s">
         <v>312</v>
@@ -4370,22 +4373,22 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B122" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="C122" t="s">
-        <v>179</v>
+        <v>267</v>
       </c>
       <c r="D122" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="E122" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="F122" t="s">
-        <v>1</v>
+        <v>315</v>
       </c>
       <c r="G122">
         <v>1</v>
@@ -4393,7 +4396,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B123" t="s">
         <v>320</v>
@@ -4416,22 +4419,22 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>171</v>
+        <v>323</v>
       </c>
       <c r="B124" t="s">
-        <v>172</v>
+        <v>320</v>
       </c>
       <c r="C124" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D124" t="s">
-        <v>174</v>
+        <v>321</v>
       </c>
       <c r="E124" t="s">
-        <v>172</v>
+        <v>322</v>
       </c>
       <c r="F124" t="s">
-        <v>175</v>
+        <v>1</v>
       </c>
       <c r="G124">
         <v>1</v>
@@ -4439,22 +4442,22 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>52</v>
+        <v>171</v>
       </c>
       <c r="B125" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="C125" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D125" t="s">
-        <v>106</v>
+        <v>174</v>
       </c>
       <c r="E125" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="F125" t="s">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="G125">
         <v>1</v>
@@ -4462,22 +4465,22 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B126" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
       <c r="C126" t="s">
-        <v>324</v>
+        <v>181</v>
       </c>
       <c r="D126" t="s">
-        <v>325</v>
+        <v>106</v>
       </c>
       <c r="E126" t="s">
-        <v>326</v>
+        <v>107</v>
       </c>
       <c r="F126" t="s">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G126">
         <v>1</v>
@@ -4485,7 +4488,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B127" t="s">
         <v>93</v>
@@ -4508,22 +4511,22 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>327</v>
+        <v>40</v>
       </c>
       <c r="B128" t="s">
         <v>93</v>
       </c>
       <c r="C128" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D128" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E128" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F128" t="s">
-        <v>331</v>
+        <v>1</v>
       </c>
       <c r="G128">
         <v>1</v>
@@ -4531,7 +4534,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B129" t="s">
         <v>93</v>
@@ -4554,19 +4557,19 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B130" t="s">
-        <v>334</v>
+        <v>93</v>
       </c>
       <c r="C130" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="D130" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="E130" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="F130" t="s">
         <v>331</v>
@@ -4577,22 +4580,22 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>53</v>
+        <v>333</v>
       </c>
       <c r="B131" t="s">
-        <v>111</v>
+        <v>334</v>
       </c>
       <c r="C131" t="s">
-        <v>112</v>
+        <v>335</v>
       </c>
       <c r="D131" t="s">
-        <v>113</v>
+        <v>336</v>
       </c>
       <c r="E131" t="s">
-        <v>111</v>
+        <v>337</v>
       </c>
       <c r="F131" t="s">
-        <v>114</v>
+        <v>331</v>
       </c>
       <c r="G131">
         <v>1</v>
@@ -4600,22 +4603,22 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B132" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C132" t="s">
-        <v>192</v>
+        <v>112</v>
       </c>
       <c r="D132" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="E132" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="F132" t="s">
-        <v>1</v>
+        <v>114</v>
       </c>
       <c r="G132">
         <v>1</v>
@@ -4623,7 +4626,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B133" t="s">
         <v>93</v>
@@ -4646,22 +4649,22 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>338</v>
+        <v>44</v>
       </c>
       <c r="B134" t="s">
-        <v>339</v>
+        <v>93</v>
       </c>
       <c r="C134" t="s">
-        <v>340</v>
+        <v>192</v>
       </c>
       <c r="D134" t="s">
-        <v>341</v>
+        <v>94</v>
       </c>
       <c r="E134" t="s">
-        <v>342</v>
+        <v>95</v>
       </c>
       <c r="F134" t="s">
-        <v>343</v>
+        <v>1</v>
       </c>
       <c r="G134">
         <v>1</v>
@@ -4669,22 +4672,22 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>205</v>
+        <v>338</v>
       </c>
       <c r="B135" t="s">
-        <v>206</v>
+        <v>339</v>
       </c>
       <c r="C135" t="s">
-        <v>207</v>
+        <v>340</v>
       </c>
       <c r="D135" t="s">
-        <v>380</v>
+        <v>341</v>
       </c>
       <c r="E135" t="s">
-        <v>380</v>
+        <v>342</v>
       </c>
       <c r="F135" t="s">
-        <v>381</v>
+        <v>343</v>
       </c>
       <c r="G135">
         <v>1</v>
@@ -4692,22 +4695,22 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>161</v>
+        <v>205</v>
       </c>
       <c r="B136" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C136" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D136" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E136" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F136" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G136">
         <v>1</v>
@@ -4715,7 +4718,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B137" t="s">
         <v>200</v>
@@ -4738,7 +4741,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="B138" t="s">
         <v>200</v>
@@ -4761,7 +4764,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B139" t="s">
         <v>200</v>
@@ -4784,22 +4787,22 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>344</v>
+        <v>202</v>
       </c>
       <c r="B140" t="s">
-        <v>345</v>
+        <v>200</v>
       </c>
       <c r="C140" t="s">
-        <v>346</v>
+        <v>211</v>
       </c>
       <c r="D140" t="s">
-        <v>347</v>
+        <v>382</v>
       </c>
       <c r="E140" t="s">
-        <v>348</v>
+        <v>383</v>
       </c>
       <c r="F140" t="s">
-        <v>349</v>
+        <v>384</v>
       </c>
       <c r="G140">
         <v>1</v>
@@ -4807,22 +4810,22 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>203</v>
+        <v>344</v>
       </c>
       <c r="B141" t="s">
-        <v>204</v>
+        <v>345</v>
       </c>
       <c r="C141" t="s">
-        <v>199</v>
+        <v>346</v>
       </c>
       <c r="D141" t="s">
-        <v>385</v>
+        <v>347</v>
       </c>
       <c r="E141" t="s">
-        <v>386</v>
+        <v>348</v>
       </c>
       <c r="F141" t="s">
-        <v>387</v>
+        <v>349</v>
       </c>
       <c r="G141">
         <v>1</v>
@@ -4830,22 +4833,22 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>350</v>
+        <v>203</v>
       </c>
       <c r="B142" t="s">
-        <v>351</v>
+        <v>204</v>
       </c>
       <c r="C142" t="s">
-        <v>346</v>
+        <v>199</v>
       </c>
       <c r="D142" t="s">
-        <v>352</v>
+        <v>385</v>
       </c>
       <c r="E142" t="s">
-        <v>351</v>
+        <v>386</v>
       </c>
       <c r="F142" t="s">
-        <v>353</v>
+        <v>387</v>
       </c>
       <c r="G142">
         <v>1</v>
@@ -4853,22 +4856,22 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B143" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C143" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="D143" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="E143" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="F143" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="G143">
         <v>1</v>
@@ -4876,22 +4879,22 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B144" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C144" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="D144" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="E144" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="F144" t="s">
-        <v>20</v>
+        <v>359</v>
       </c>
       <c r="G144">
         <v>1</v>
@@ -4899,22 +4902,22 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>138</v>
+        <v>360</v>
       </c>
       <c r="B145" t="s">
-        <v>139</v>
+        <v>361</v>
       </c>
       <c r="C145" t="s">
-        <v>140</v>
+        <v>362</v>
       </c>
       <c r="D145" t="s">
-        <v>141</v>
+        <v>363</v>
       </c>
       <c r="E145" t="s">
-        <v>142</v>
+        <v>364</v>
       </c>
       <c r="F145" t="s">
-        <v>143</v>
+        <v>20</v>
       </c>
       <c r="G145">
         <v>1</v>
@@ -4922,22 +4925,22 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="B146" t="s">
-        <v>9</v>
+        <v>139</v>
       </c>
       <c r="C146" t="s">
-        <v>365</v>
+        <v>140</v>
       </c>
       <c r="D146" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="E146" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="F146" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="G146">
         <v>1</v>
@@ -4945,7 +4948,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>366</v>
+        <v>58</v>
       </c>
       <c r="B147" t="s">
         <v>9</v>
@@ -4968,24 +4971,47 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>366</v>
+      </c>
+      <c r="B148" t="s">
+        <v>9</v>
+      </c>
+      <c r="C148" t="s">
+        <v>365</v>
+      </c>
+      <c r="D148" t="s">
+        <v>163</v>
+      </c>
+      <c r="E148" t="s">
+        <v>164</v>
+      </c>
+      <c r="F148" t="s">
+        <v>10</v>
+      </c>
+      <c r="G148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>212</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B149" t="s">
         <v>213</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C149" t="s">
         <v>214</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D149" t="s">
         <v>388</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E149" t="s">
         <v>389</v>
       </c>
-      <c r="F148" t="s">
+      <c r="F149" t="s">
         <v>390</v>
       </c>
-      <c r="G148">
+      <c r="G149">
         <v>1</v>
       </c>
     </row>

</xml_diff>